<commit_message>
Overwritten with clean code and data from Lizzie
</commit_message>
<xml_diff>
--- a/Reversal cFos cohort blind.xlsx
+++ b/Reversal cFos cohort blind.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/localadmin/code/rev_fos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lizzie\Documents\GitHub\SAPAP3_reversal\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EB7FDA-21F1-4B61-A2EB-D45A119B6130}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="18820" windowHeight="7060"/>
+    <workbookView xWindow="315" yWindow="465" windowWidth="18825" windowHeight="7065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -97,13 +98,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -116,6 +116,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -407,241 +410,269 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>379</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>390</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>402</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>403</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1844</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>1846</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1853</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>1854</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>1860</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>1870</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>1878</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>1896</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>1897</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>1901</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
         <v>1906</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
         <v>1907</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
         <v>1909</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
         <v>1917</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
         <v>1927</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
         <v>1932</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
         <v>2001</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
         <v>2010</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>2015</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>2019</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>2021</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>2022</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>2023</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -649,24 +680,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>